<commit_message>
First draft entered into PDF for submission to FMC
</commit_message>
<xml_diff>
--- a/fundraising/2017-10 AMOSO Innovation fund/Innovation Fund Budget.xlsx
+++ b/fundraising/2017-10 AMOSO Innovation fund/Innovation Fund Budget.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -256,6 +256,9 @@
     <t xml:space="preserve">Alex Pavlosky, Research Assistant, avg 5 hrs/week </t>
   </si>
   <si>
+    <t xml:space="preserve">Luka Mustafa, Electronics Engineer, avg 10hrs/week</t>
+  </si>
+  <si>
     <t xml:space="preserve">Subtotal - Staff Compensation - C</t>
   </si>
   <si>
@@ -282,7 +285,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Luka Mustafa, Contracted Engineer, as needed</t>
+    <t xml:space="preserve">Luka Mustafa, Engineer, avg 10hrs/week</t>
   </si>
   <si>
     <t xml:space="preserve">Melanie Columbus, Research Coordinator, Division of Emergency Medicine, x1/2 day per week</t>
@@ -380,7 +383,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1 Supplies (Innovation Fund) –  </t>
+    <t xml:space="preserve">1 Supplies (Innovation Fund) –  Prototype pulse oximeter devices ($500 x 10 units)</t>
   </si>
   <si>
     <t xml:space="preserve">2 Supplies (Other Funding) – Raw material (plastic resin &amp; plastic filament), printer parts</t>
@@ -389,7 +392,7 @@
     <t xml:space="preserve">3 Equipment (Other Funding) – FDM 3D printers (3 x Prusa i3 MK2), SLA 3D printer (1 x Form Labs Form2)</t>
   </si>
   <si>
-    <t xml:space="preserve">4 Other Expenses (Innovation Fund) – Meetings (travel &amp; accomodation)</t>
+    <t xml:space="preserve">4 Other Expenses (Innovation Fund) – Meetings (travel &amp; accommodation)</t>
   </si>
   <si>
     <t xml:space="preserve">5 Other Expenses (Other Source Funding) – accounting, mail &amp; postage</t>
@@ -446,7 +449,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="39">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -468,6 +471,80 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -651,12 +728,54 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -667,28 +786,43 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF404040"/>
-        <bgColor rgb="FF333300"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF7EB3E3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -741,7 +875,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -767,77 +901,125 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="11" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -845,152 +1027,168 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="5" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="12" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="5" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="25" fillId="12" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1015,7 +1213,7 @@
       <rgbColor rgb="FF7EB3E3"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF62B3DC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1027,11 +1225,11 @@
       <rgbColor rgb="FF17375E"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF404040"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1042,17 +1240,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="92.5074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81851851851852"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1361,53 +1559,55 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="24" t="n">
-        <f aca="false">SUM(B29:B31)</f>
-        <v>69962.5</v>
-      </c>
-      <c r="C32" s="24" t="n">
-        <f aca="false">SUM(C29:C31)</f>
-        <v>69962.5</v>
+      <c r="B32" s="23" t="n">
+        <v>7500</v>
+      </c>
+      <c r="C32" s="23" t="n">
+        <v>7500</v>
       </c>
       <c r="D32" s="24" t="n">
         <f aca="false">SUM(B32:C32)</f>
-        <v>139925</v>
-      </c>
-    </row>
-    <row r="33" s="18" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-    </row>
-    <row r="34" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B33" s="24" t="n">
+        <f aca="false">SUM(B30:B32)</f>
+        <v>77462.5</v>
+      </c>
+      <c r="C33" s="24" t="n">
+        <f aca="false">SUM(C30:C32)</f>
+        <v>77462.5</v>
+      </c>
+      <c r="D33" s="24" t="n">
+        <f aca="false">SUM(B33:C33)</f>
+        <v>154925</v>
+      </c>
+    </row>
+    <row r="34" s="18" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+    </row>
+    <row r="35" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C35" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="23" t="n">
-        <v>7500</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24" t="n">
-        <f aca="false">SUM(B35:C35)</f>
-        <v>7500</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1415,97 +1615,97 @@
         <v>32</v>
       </c>
       <c r="B36" s="23" t="n">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="C36" s="23" t="n">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="D36" s="24" t="n">
         <f aca="false">SUM(B36:C36)</f>
-        <v>0</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="24" t="n">
-        <f aca="false">SUM(B34:B36)</f>
-        <v>7500</v>
-      </c>
-      <c r="C37" s="24" t="n">
-        <f aca="false">SUM(C34:C36)</f>
-        <v>0</v>
+      <c r="B37" s="23" t="n">
+        <v>6855</v>
+      </c>
+      <c r="C37" s="23" t="n">
+        <v>6855</v>
       </c>
       <c r="D37" s="24" t="n">
         <f aca="false">SUM(B37:C37)</f>
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-    </row>
-    <row r="39" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26" t="s">
+        <v>13710</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="35" t="n">
-        <f aca="false">SUM(B22+B27+B32+B37)</f>
-        <v>175712.5</v>
-      </c>
-      <c r="C39" s="35" t="n">
-        <f aca="false">SUM(C22+C27+C32+C37)</f>
-        <v>168212.5</v>
-      </c>
-      <c r="D39" s="35" t="n">
-        <f aca="false">SUM(D22+D27+D32+D37)</f>
-        <v>343925</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="36"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-    </row>
-    <row r="41" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19" t="s">
+      <c r="B38" s="24" t="n">
+        <f aca="false">SUM(B35:B37)</f>
+        <v>18855</v>
+      </c>
+      <c r="C38" s="24" t="n">
+        <f aca="false">SUM(C35:C37)</f>
+        <v>18855</v>
+      </c>
+      <c r="D38" s="24" t="n">
+        <f aca="false">SUM(B38:C38)</f>
+        <v>37710</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="32"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+    </row>
+    <row r="40" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B40" s="35" t="n">
+        <f aca="false">SUM(B22+B27+B33+B38)</f>
+        <v>194567.5</v>
+      </c>
+      <c r="C40" s="35" t="n">
+        <f aca="false">SUM(C22+C27+C33+C38)</f>
+        <v>194567.5</v>
+      </c>
+      <c r="D40" s="35" t="n">
+        <f aca="false">SUM(D22+D27+D33+D38)</f>
+        <v>389135</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+    </row>
+    <row r="42" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C42" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D42" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24" t="n">
-        <f aca="false">SUM(B42:C42)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="43" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="23" t="n">
-        <v>0</v>
-      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="24" t="n">
         <f aca="false">SUM(B43:C43)</f>
         <v>0</v>
@@ -1516,81 +1716,81 @@
         <v>38</v>
       </c>
       <c r="B44" s="23" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="C44" s="23" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D44" s="24" t="n">
         <f aca="false">SUM(B44:C44)</f>
-        <v>3000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="24" t="n">
-        <f aca="false">SUM(B42:B44)</f>
-        <v>1000</v>
-      </c>
-      <c r="C45" s="24" t="n">
-        <f aca="false">SUM(C42:C44)</f>
+      <c r="B45" s="23" t="n">
+        <v>4400</v>
+      </c>
+      <c r="C45" s="23" t="n">
         <v>2000</v>
       </c>
       <c r="D45" s="24" t="n">
         <f aca="false">SUM(B45:C45)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="32"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-    </row>
-    <row r="47" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19" t="s">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B46" s="24" t="n">
+        <f aca="false">SUM(B43:B45)</f>
+        <v>9400</v>
+      </c>
+      <c r="C46" s="24" t="n">
+        <f aca="false">SUM(C43:C45)</f>
+        <v>2000</v>
+      </c>
+      <c r="D46" s="24" t="n">
+        <f aca="false">SUM(B46:C46)</f>
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="32"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+    </row>
+    <row r="48" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C48" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D48" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="23" t="n">
+    <row r="49" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="23" t="n">
         <v>600</v>
       </c>
-      <c r="C48" s="23" t="n">
+      <c r="C49" s="23" t="n">
         <v>1200</v>
-      </c>
-      <c r="D48" s="24" t="n">
-        <f aca="false">SUM(B48:C48)</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="23" t="n">
-        <v>8500</v>
-      </c>
-      <c r="C49" s="23" t="n">
-        <v>500</v>
       </c>
       <c r="D49" s="24" t="n">
         <f aca="false">SUM(B49:C49)</f>
-        <v>9000</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1598,94 +1798,101 @@
         <v>38</v>
       </c>
       <c r="B50" s="23" t="n">
-        <v>2000</v>
+        <v>8500</v>
       </c>
       <c r="C50" s="23" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D50" s="24" t="n">
         <f aca="false">SUM(B50:C50)</f>
-        <v>4000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="24" t="n">
-        <f aca="false">SUM(B48:B50)</f>
-        <v>11100</v>
-      </c>
-      <c r="C51" s="24" t="n">
-        <f aca="false">SUM(C48:C50)</f>
-        <v>3700</v>
+      <c r="A51" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="23" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C51" s="23" t="n">
+        <v>2000</v>
       </c>
       <c r="D51" s="24" t="n">
         <f aca="false">SUM(B51:C51)</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="24" t="n">
+        <f aca="false">SUM(B49:B51)</f>
+        <v>11100</v>
+      </c>
+      <c r="C52" s="24" t="n">
+        <f aca="false">SUM(C49:C51)</f>
+        <v>3700</v>
+      </c>
+      <c r="D52" s="24" t="n">
+        <f aca="false">SUM(B52:C52)</f>
         <v>14800</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="32"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-    </row>
-    <row r="53" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="35" t="n">
-        <f aca="false">B39+B45+B51</f>
-        <v>187812.5</v>
-      </c>
-      <c r="C53" s="35" t="n">
-        <f aca="false">C39+C45+C51</f>
-        <v>173912.5</v>
-      </c>
-      <c r="D53" s="35" t="n">
-        <f aca="false">D39+D45+D51</f>
-        <v>361725</v>
-      </c>
+    <row r="53" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="32"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
     </row>
     <row r="54" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="35" t="n">
-        <f aca="false">SUM(B22+B32+B45)</f>
-        <v>70962.5</v>
+        <f aca="false">B40+B46+B52</f>
+        <v>215067.5</v>
       </c>
       <c r="C54" s="35" t="n">
-        <f aca="false">SUM(C22+C32+C45)</f>
-        <v>71962.5</v>
+        <f aca="false">C40+C46+C52</f>
+        <v>200267.5</v>
       </c>
       <c r="D54" s="35" t="n">
-        <f aca="false">SUM(D22+D32+D45)</f>
-        <v>142925</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="32"/>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-    </row>
-    <row r="56" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="40" t="s">
+        <f aca="false">D40+D46+D52</f>
+        <v>415335</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-    </row>
-    <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="41" t="s">
+      <c r="B55" s="35" t="n">
+        <f aca="false">SUM(B22+B33+B46)</f>
+        <v>86862.5</v>
+      </c>
+      <c r="C55" s="35" t="n">
+        <f aca="false">SUM(C22+C33+C46)</f>
+        <v>79462.5</v>
+      </c>
+      <c r="D55" s="35" t="n">
+        <f aca="false">SUM(D22+D33+D46)</f>
+        <v>166325</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="32"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+    </row>
+    <row r="57" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="41"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="41" t="s">
@@ -1696,20 +1903,20 @@
       <c r="D58" s="41"/>
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="42" t="s">
+      <c r="A59" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="41" t="s">
@@ -1719,40 +1926,42 @@
       <c r="C61" s="41"/>
       <c r="D61" s="41"/>
     </row>
-    <row r="62" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-    </row>
-    <row r="63" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="15" t="s">
+    <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-    </row>
-    <row r="64" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="45" t="s">
+      <c r="B62" s="41"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+    </row>
+    <row r="63" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+    </row>
+    <row r="64" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+    </row>
+    <row r="65" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C64" s="45" t="s">
+      <c r="B65" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D64" s="45"/>
-    </row>
-    <row r="65" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="46"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
+      <c r="C65" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="45"/>
     </row>
     <row r="66" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="48"/>
+      <c r="A66" s="46"/>
       <c r="B66" s="23"/>
       <c r="C66" s="47"/>
       <c r="D66" s="47"/>
@@ -1763,6 +1972,13 @@
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
     </row>
+    <row r="68" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="48"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="A1:A2"/>
@@ -1782,16 +1998,16 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A59:D59"/>
     <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A64:D64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.28125" bottom="0.279861111111111" header="0.3" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
draft upload, mostly filled, for FMC deadline
</commit_message>
<xml_diff>
--- a/fundraising/2017-10 AMOSO Innovation fund/Innovation Fund Budget.xlsx
+++ b/fundraising/2017-10 AMOSO Innovation fund/Innovation Fund Budget.xlsx
@@ -383,7 +383,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1 Supplies (Innovation Fund) –  Prototype pulse oximeter devices ($500 x 10 units)</t>
+    <t xml:space="preserve">1 Equipment (Innovation Fund) –  Prototype pulse oximeter devices ($500 x 10 units)</t>
   </si>
   <si>
     <t xml:space="preserve">2 Supplies (Other Funding) – Raw material (plastic resin &amp; plastic filament), printer parts</t>
@@ -449,7 +449,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -471,80 +471,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -728,54 +654,12 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -786,43 +670,28 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF404040"/>
-        <bgColor rgb="FF333333"/>
+        <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor rgb="FF7EB3E3"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -875,7 +744,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -901,125 +770,77 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="11" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,168 +848,152 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="12" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="12" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="5" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1213,7 +1018,7 @@
       <rgbColor rgb="FF7EB3E3"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF62B3DC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1225,11 +1030,11 @@
       <rgbColor rgb="FF17375E"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF404040"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1242,15 +1047,15 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.82"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.8592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>